<commit_message>
Adult pax name update
</commit_message>
<xml_diff>
--- a/HybirdFramework/TestData/Data.xlsx
+++ b/HybirdFramework/TestData/Data.xlsx
@@ -94,7 +94,7 @@
     <t>Firstname</t>
   </si>
   <si>
-    <t>Tamil Babar</t>
+    <t>Tamil irfan</t>
   </si>
   <si>
     <t>Lastname</t>
@@ -1279,7 +1279,7 @@
   <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="2"/>

</xml_diff>

<commit_message>
adding the Listner class
</commit_message>
<xml_diff>
--- a/HybirdFramework/TestData/Data.xlsx
+++ b/HybirdFramework/TestData/Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12300" activeTab="1"/>
+    <workbookView windowWidth="28800" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="55">
   <si>
     <t>Trip</t>
   </si>
@@ -94,7 +94,7 @@
     <t>Firstname</t>
   </si>
   <si>
-    <t>Tamil hasan</t>
+    <t>Tamil</t>
   </si>
   <si>
     <t>Lastname</t>
@@ -125,9 +125,6 @@
   </si>
   <si>
     <t>Mstr.</t>
-  </si>
-  <si>
-    <t>Tamil</t>
   </si>
   <si>
     <t>dob date</t>
@@ -1156,7 +1153,7 @@
   <sheetPr/>
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -1204,7 +1201,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="1">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1278,8 +1275,8 @@
   <sheetPr/>
   <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="2"/>
@@ -1384,7 +1381,7 @@
         <v>20</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="C12" s="2"/>
     </row>
@@ -1399,28 +1396,28 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>33</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>34</v>
       </c>
       <c r="C14" s="2"/>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>35</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>36</v>
       </c>
       <c r="C15" s="2"/>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" s="3" t="s">
         <v>37</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>38</v>
       </c>
       <c r="C16" s="2"/>
     </row>
@@ -1440,7 +1437,7 @@
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -1459,7 +1456,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C21" s="2"/>
     </row>
@@ -1474,28 +1471,28 @@
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C23" s="2"/>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C24" s="2"/>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C25" s="2"/>
     </row>
@@ -1539,23 +1536,23 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" s="7" t="s">
         <v>45</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B4" s="3">
         <v>123</v>
@@ -1567,15 +1564,15 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>23</v>
@@ -1583,23 +1580,23 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>50</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>52</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B10" s="3">
         <v>641001</v>
@@ -1607,7 +1604,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B11" s="3">
         <v>9876543210</v>

</xml_diff>

<commit_message>
Adding Listeners class and Screenshot shot only for failed case .
</commit_message>
<xml_diff>
--- a/HybirdFramework/TestData/Data.xlsx
+++ b/HybirdFramework/TestData/Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12300"/>
+    <workbookView windowWidth="28800" windowHeight="12300" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="57">
   <si>
     <t>Trip</t>
   </si>
@@ -94,73 +94,79 @@
     <t>Firstname</t>
   </si>
   <si>
+    <t>Tamil Yadav</t>
+  </si>
+  <si>
+    <t>Lastname</t>
+  </si>
+  <si>
+    <t>GQ</t>
+  </si>
+  <si>
+    <t>MobileNo</t>
+  </si>
+  <si>
+    <t>EMail</t>
+  </si>
+  <si>
+    <t>lingeswar@goquo.com</t>
+  </si>
+  <si>
+    <t>Confirmmail</t>
+  </si>
+  <si>
+    <t>Residential</t>
+  </si>
+  <si>
+    <t>2000-BARANGAROO,NSW</t>
+  </si>
+  <si>
+    <t>Pax 2</t>
+  </si>
+  <si>
+    <t>Mstr.</t>
+  </si>
+  <si>
+    <t>Lingeswar</t>
+  </si>
+  <si>
+    <t>dob date</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>DOB Month</t>
+  </si>
+  <si>
+    <t>May</t>
+  </si>
+  <si>
+    <t>DOB Year</t>
+  </si>
+  <si>
+    <t>2016</t>
+  </si>
+  <si>
+    <t>Pax 3</t>
+  </si>
+  <si>
+    <t>Satheesh</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>July</t>
+  </si>
+  <si>
+    <t>2023</t>
+  </si>
+  <si>
+    <t>Paymentcardname</t>
+  </si>
+  <si>
     <t>Tamil</t>
-  </si>
-  <si>
-    <t>Lastname</t>
-  </si>
-  <si>
-    <t>GQ</t>
-  </si>
-  <si>
-    <t>MobileNo</t>
-  </si>
-  <si>
-    <t>EMail</t>
-  </si>
-  <si>
-    <t>lingeswar@goquo.com</t>
-  </si>
-  <si>
-    <t>Confirmmail</t>
-  </si>
-  <si>
-    <t>Residential</t>
-  </si>
-  <si>
-    <t>2000-BARANGAROO,NSW</t>
-  </si>
-  <si>
-    <t>Pax 2</t>
-  </si>
-  <si>
-    <t>Mstr.</t>
-  </si>
-  <si>
-    <t>dob date</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>DOB Month</t>
-  </si>
-  <si>
-    <t>May</t>
-  </si>
-  <si>
-    <t>DOB Year</t>
-  </si>
-  <si>
-    <t>2016</t>
-  </si>
-  <si>
-    <t>Pax 3</t>
-  </si>
-  <si>
-    <t>Satheesh</t>
-  </si>
-  <si>
-    <t>23</t>
-  </si>
-  <si>
-    <t>July</t>
-  </si>
-  <si>
-    <t>2023</t>
-  </si>
-  <si>
-    <t>Paymentcardname</t>
   </si>
   <si>
     <t>Cardno</t>
@@ -1153,8 +1159,8 @@
   <sheetPr/>
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="2"/>
@@ -1275,8 +1281,8 @@
   <sheetPr/>
   <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="2"/>
@@ -1381,7 +1387,7 @@
         <v>20</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="C12" s="2"/>
     </row>
@@ -1396,28 +1402,28 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C14" s="2"/>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C15" s="2"/>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C16" s="2"/>
     </row>
@@ -1437,7 +1443,7 @@
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -1456,7 +1462,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C21" s="2"/>
     </row>
@@ -1471,28 +1477,28 @@
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C23" s="2"/>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C24" s="2"/>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C25" s="2"/>
     </row>
@@ -1536,23 +1542,23 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>21</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B4" s="3">
         <v>123</v>
@@ -1564,15 +1570,15 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>21</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>23</v>
@@ -1580,23 +1586,23 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B10" s="3">
         <v>641001</v>
@@ -1604,7 +1610,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B11" s="3">
         <v>9876543210</v>

</xml_diff>

<commit_message>
Adding Parameter in Month and date
</commit_message>
<xml_diff>
--- a/HybirdFramework/TestData/Data.xlsx
+++ b/HybirdFramework/TestData/Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12300"/>
+    <workbookView windowWidth="28800" windowHeight="12300" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -94,7 +94,7 @@
     <t>Firstname</t>
   </si>
   <si>
-    <t>TamilKumaran</t>
+    <t>ASASAS</t>
   </si>
   <si>
     <t>Lastname</t>
@@ -1160,8 +1160,8 @@
   <sheetPr/>
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="2"/>
@@ -1285,8 +1285,8 @@
   <sheetPr/>
   <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B26" sqref="A1:B26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="2"/>

</xml_diff>

<commit_message>
Update Pax selection for 2 Adult , 1 child , 1Infant
</commit_message>
<xml_diff>
--- a/HybirdFramework/TestData/Data.xlsx
+++ b/HybirdFramework/TestData/Data.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12300"/>
+    <workbookView windowWidth="28800" windowHeight="12300" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Paxdetails" sheetId="2" r:id="rId2"/>
     <sheet name="Payment" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="65">
   <si>
     <t>Trip</t>
   </si>
@@ -82,7 +82,7 @@
     <t>pro select_out</t>
   </si>
   <si>
-    <t>Pax 1</t>
+    <t>Mainpax</t>
   </si>
   <si>
     <t>Title</t>
@@ -121,6 +121,9 @@
     <t>2000-BARANGAROO,NSW</t>
   </si>
   <si>
+    <t>Childpax</t>
+  </si>
+  <si>
     <t>Pax 2</t>
   </si>
   <si>
@@ -148,10 +151,13 @@
     <t>2016</t>
   </si>
   <si>
+    <t>Infantpax</t>
+  </si>
+  <si>
     <t>Pax 3</t>
   </si>
   <si>
-    <t>Satheesh</t>
+    <t>Parvin</t>
   </si>
   <si>
     <t>23</t>
@@ -161,6 +167,12 @@
   </si>
   <si>
     <t>2023</t>
+  </si>
+  <si>
+    <t>2Adultpax</t>
+  </si>
+  <si>
+    <t>Pradeep</t>
   </si>
   <si>
     <t>Paymentcardname</t>
@@ -224,8 +236,16 @@
     <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="21">
-    <font>
+  <fonts count="22">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -701,137 +721,137 @@
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -840,13 +860,15 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" quotePrefix="1">
       <alignment horizontal="left"/>
@@ -1172,7 +1194,7 @@
   <sheetPr/>
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
@@ -1186,10 +1208,10 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6"/>
+      <c r="C1" s="8"/>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
@@ -1264,10 +1286,10 @@
       </c>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="9" t="s">
         <v>16</v>
       </c>
       <c r="C12" s="2"/>
@@ -1295,10 +1317,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A28" sqref="$A28:$XFD28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="2"/>
@@ -1308,7 +1330,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B1" s="2"/>
@@ -1354,7 +1376,7 @@
       <c r="A6" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="5" t="s">
         <v>26</v>
       </c>
       <c r="C6" s="2"/>
@@ -1363,7 +1385,7 @@
       <c r="A7" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="5" t="s">
         <v>26</v>
       </c>
       <c r="C7" s="2"/>
@@ -1378,13 +1400,15 @@
       <c r="C8" s="2"/>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="2"/>
+      <c r="A9" s="4" t="s">
+        <v>30</v>
+      </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -1394,7 +1418,7 @@
         <v>18</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C11" s="2"/>
     </row>
@@ -1403,7 +1427,7 @@
         <v>20</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C12" s="2"/>
     </row>
@@ -1418,28 +1442,28 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C14" s="2"/>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C15" s="2"/>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C16" s="2"/>
     </row>
@@ -1453,13 +1477,15 @@
       <c r="C17" s="2"/>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" s="2"/>
+      <c r="A18" s="4" t="s">
+        <v>40</v>
+      </c>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -1469,7 +1495,7 @@
         <v>18</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C20" s="2"/>
     </row>
@@ -1478,7 +1504,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C21" s="2"/>
     </row>
@@ -1493,28 +1519,28 @@
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C23" s="2"/>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C24" s="2"/>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C25" s="2"/>
     </row>
@@ -1526,6 +1552,44 @@
         <v>29</v>
       </c>
       <c r="C26" s="2"/>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C31" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1558,23 +1622,23 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>47</v>
+        <v>50</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="2" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="B4" s="3">
         <v>123</v>
@@ -1586,15 +1650,15 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>49</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="2" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>23</v>
@@ -1602,23 +1666,23 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="2" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="2" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="2" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B10" s="3">
         <v>641001</v>
@@ -1626,7 +1690,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="2" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B11" s="3">
         <v>9876543210</v>
@@ -1634,18 +1698,18 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="2" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="2" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
     </row>
     <row r="14" spans="1:2">

</xml_diff>